<commit_message>
Added first working version of MSCExtractor
</commit_message>
<xml_diff>
--- a/data/MSC Port Code Mapping.xlsx
+++ b/data/MSC Port Code Mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tym.Teo\Documents\Delay Report - Rewrite\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E890928-06E6-43D9-9FCF-C37E5AB31239}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C44ACA18-95A2-4143-9DF4-86C95636C7CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4779,15 +4779,9 @@
     <t>TWKEL</t>
   </si>
   <si>
-    <t>KEELUNG, Taiwain (China)</t>
-  </si>
-  <si>
     <t>TWKHH</t>
   </si>
   <si>
-    <t>KAOHSIUNG, Taiwain (China)</t>
-  </si>
-  <si>
     <t>TWTPE</t>
   </si>
   <si>
@@ -4797,9 +4791,6 @@
     <t>TWTXG</t>
   </si>
   <si>
-    <t>TAICHUNG, Taiwain (China)</t>
-  </si>
-  <si>
     <t>TWTYN</t>
   </si>
   <si>
@@ -5362,6 +5353,15 @@
   </si>
   <si>
     <t>COEGA, South Africa</t>
+  </si>
+  <si>
+    <t>KAOHSIUNG, China</t>
+  </si>
+  <si>
+    <t>KEELUNG, China</t>
+  </si>
+  <si>
+    <t>TAICHUNG, China</t>
   </si>
 </sst>
 </file>
@@ -5749,8 +5749,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B896"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A778" workbookViewId="0">
+      <selection activeCell="B802" sqref="B802"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12149,783 +12149,783 @@
         <v>1583</v>
       </c>
       <c r="B799" s="3" t="s">
-        <v>1584</v>
+        <v>1777</v>
       </c>
     </row>
     <row r="800" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A800" s="3" t="s">
-        <v>1585</v>
+        <v>1584</v>
       </c>
       <c r="B800" s="3" t="s">
-        <v>1586</v>
+        <v>1776</v>
       </c>
     </row>
     <row r="801" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A801" s="4" t="s">
-        <v>1587</v>
+        <v>1585</v>
       </c>
       <c r="B801" s="4" t="s">
-        <v>1588</v>
+        <v>1586</v>
       </c>
     </row>
     <row r="802" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A802" s="3" t="s">
-        <v>1589</v>
+        <v>1587</v>
       </c>
       <c r="B802" s="3" t="s">
-        <v>1590</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="803" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A803" s="4" t="s">
-        <v>1591</v>
+        <v>1588</v>
       </c>
       <c r="B803" s="4" t="s">
-        <v>1592</v>
+        <v>1589</v>
       </c>
     </row>
     <row r="804" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A804" s="3" t="s">
-        <v>1593</v>
+        <v>1590</v>
       </c>
       <c r="B804" s="3" t="s">
-        <v>1594</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="805" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A805" s="3" t="s">
-        <v>1595</v>
+        <v>1592</v>
       </c>
       <c r="B805" s="3" t="s">
-        <v>1596</v>
+        <v>1593</v>
       </c>
     </row>
     <row r="806" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A806" s="3" t="s">
-        <v>1597</v>
+        <v>1594</v>
       </c>
       <c r="B806" s="3" t="s">
-        <v>1598</v>
+        <v>1595</v>
       </c>
     </row>
     <row r="807" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A807" s="3" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="B807" s="3" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="808" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A808" s="3" t="s">
-        <v>1601</v>
+        <v>1598</v>
       </c>
       <c r="B808" s="3" t="s">
-        <v>1602</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="809" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A809" s="3" t="s">
-        <v>1603</v>
+        <v>1600</v>
       </c>
       <c r="B809" s="3" t="s">
-        <v>1604</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="810" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A810" s="3" t="s">
-        <v>1605</v>
+        <v>1602</v>
       </c>
       <c r="B810" s="3" t="s">
-        <v>1606</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="811" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A811" s="3" t="s">
-        <v>1607</v>
+        <v>1604</v>
       </c>
       <c r="B811" s="3" t="s">
-        <v>1608</v>
+        <v>1605</v>
       </c>
     </row>
     <row r="812" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A812" s="3" t="s">
-        <v>1609</v>
+        <v>1606</v>
       </c>
       <c r="B812" s="3" t="s">
-        <v>1610</v>
+        <v>1607</v>
       </c>
     </row>
     <row r="813" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A813" s="3" t="s">
-        <v>1611</v>
+        <v>1608</v>
       </c>
       <c r="B813" s="3" t="s">
-        <v>1612</v>
+        <v>1609</v>
       </c>
     </row>
     <row r="814" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A814" s="3" t="s">
-        <v>1613</v>
+        <v>1610</v>
       </c>
       <c r="B814" s="3" t="s">
-        <v>1614</v>
+        <v>1611</v>
       </c>
     </row>
     <row r="815" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A815" s="3" t="s">
-        <v>1615</v>
+        <v>1612</v>
       </c>
       <c r="B815" s="3" t="s">
-        <v>1616</v>
+        <v>1613</v>
       </c>
     </row>
     <row r="816" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A816" s="3" t="s">
-        <v>1617</v>
+        <v>1614</v>
       </c>
       <c r="B816" s="3" t="s">
-        <v>1618</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="817" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A817" s="3" t="s">
-        <v>1619</v>
+        <v>1616</v>
       </c>
       <c r="B817" s="3" t="s">
-        <v>1620</v>
+        <v>1617</v>
       </c>
     </row>
     <row r="818" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A818" s="4" t="s">
-        <v>1621</v>
+        <v>1618</v>
       </c>
       <c r="B818" s="4" t="s">
-        <v>1622</v>
+        <v>1619</v>
       </c>
     </row>
     <row r="819" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A819" s="3" t="s">
-        <v>1623</v>
+        <v>1620</v>
       </c>
       <c r="B819" s="3" t="s">
-        <v>1624</v>
+        <v>1621</v>
       </c>
     </row>
     <row r="820" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A820" s="3" t="s">
-        <v>1625</v>
+        <v>1622</v>
       </c>
       <c r="B820" s="3" t="s">
-        <v>1626</v>
+        <v>1623</v>
       </c>
     </row>
     <row r="821" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A821" s="3" t="s">
-        <v>1627</v>
+        <v>1624</v>
       </c>
       <c r="B821" s="3" t="s">
-        <v>1628</v>
+        <v>1625</v>
       </c>
     </row>
     <row r="822" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A822" s="3" t="s">
-        <v>1629</v>
+        <v>1626</v>
       </c>
       <c r="B822" s="3" t="s">
-        <v>1630</v>
+        <v>1627</v>
       </c>
     </row>
     <row r="823" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A823" s="3" t="s">
-        <v>1631</v>
+        <v>1628</v>
       </c>
       <c r="B823" s="3" t="s">
-        <v>1632</v>
+        <v>1629</v>
       </c>
     </row>
     <row r="824" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A824" s="3" t="s">
-        <v>1633</v>
+        <v>1630</v>
       </c>
       <c r="B824" s="3" t="s">
-        <v>1634</v>
+        <v>1631</v>
       </c>
     </row>
     <row r="825" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A825" s="3" t="s">
-        <v>1635</v>
+        <v>1632</v>
       </c>
       <c r="B825" s="3" t="s">
-        <v>1636</v>
+        <v>1633</v>
       </c>
     </row>
     <row r="826" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A826" s="3" t="s">
-        <v>1637</v>
+        <v>1634</v>
       </c>
       <c r="B826" s="3" t="s">
-        <v>1638</v>
+        <v>1635</v>
       </c>
     </row>
     <row r="827" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A827" s="3" t="s">
-        <v>1639</v>
+        <v>1636</v>
       </c>
       <c r="B827" s="3" t="s">
-        <v>1640</v>
+        <v>1637</v>
       </c>
     </row>
     <row r="828" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A828" s="4" t="s">
-        <v>1641</v>
+        <v>1638</v>
       </c>
       <c r="B828" s="4" t="s">
-        <v>1642</v>
+        <v>1639</v>
       </c>
     </row>
     <row r="829" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A829" s="3" t="s">
-        <v>1643</v>
+        <v>1640</v>
       </c>
       <c r="B829" s="3" t="s">
-        <v>1644</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="830" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A830" s="3" t="s">
-        <v>1645</v>
+        <v>1642</v>
       </c>
       <c r="B830" s="3" t="s">
-        <v>1646</v>
+        <v>1643</v>
       </c>
     </row>
     <row r="831" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A831" s="3" t="s">
-        <v>1647</v>
+        <v>1644</v>
       </c>
       <c r="B831" s="3" t="s">
-        <v>1648</v>
+        <v>1645</v>
       </c>
     </row>
     <row r="832" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A832" s="3" t="s">
-        <v>1649</v>
+        <v>1646</v>
       </c>
       <c r="B832" s="3" t="s">
-        <v>1650</v>
+        <v>1647</v>
       </c>
     </row>
     <row r="833" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A833" s="3" t="s">
-        <v>1651</v>
+        <v>1648</v>
       </c>
       <c r="B833" s="3" t="s">
-        <v>1652</v>
+        <v>1649</v>
       </c>
     </row>
     <row r="834" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A834" s="3" t="s">
-        <v>1653</v>
+        <v>1650</v>
       </c>
       <c r="B834" s="3" t="s">
-        <v>1654</v>
+        <v>1651</v>
       </c>
     </row>
     <row r="835" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A835" s="5" t="s">
-        <v>1655</v>
+        <v>1652</v>
       </c>
       <c r="B835" s="6" t="s">
-        <v>1656</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="836" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A836" s="3" t="s">
-        <v>1657</v>
+        <v>1654</v>
       </c>
       <c r="B836" s="3" t="s">
-        <v>1658</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="837" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A837" s="3" t="s">
-        <v>1659</v>
+        <v>1656</v>
       </c>
       <c r="B837" s="3" t="s">
-        <v>1660</v>
+        <v>1657</v>
       </c>
     </row>
     <row r="838" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A838" s="3" t="s">
-        <v>1661</v>
+        <v>1658</v>
       </c>
       <c r="B838" s="3" t="s">
-        <v>1662</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A839" s="3" t="s">
-        <v>1663</v>
+        <v>1660</v>
       </c>
       <c r="B839" s="3" t="s">
-        <v>1664</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A840" s="3" t="s">
-        <v>1665</v>
+        <v>1662</v>
       </c>
       <c r="B840" s="3" t="s">
-        <v>1666</v>
+        <v>1663</v>
       </c>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A841" s="7" t="s">
-        <v>1667</v>
+        <v>1664</v>
       </c>
       <c r="B841" s="7" t="s">
-        <v>1668</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A842" s="3" t="s">
-        <v>1669</v>
+        <v>1666</v>
       </c>
       <c r="B842" s="3" t="s">
-        <v>1670</v>
+        <v>1667</v>
       </c>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A843" s="3" t="s">
-        <v>1671</v>
+        <v>1668</v>
       </c>
       <c r="B843" s="3" t="s">
-        <v>1672</v>
+        <v>1669</v>
       </c>
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A844" s="3" t="s">
-        <v>1673</v>
+        <v>1670</v>
       </c>
       <c r="B844" s="3" t="s">
-        <v>1674</v>
+        <v>1671</v>
       </c>
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A845" s="3" t="s">
-        <v>1675</v>
+        <v>1672</v>
       </c>
       <c r="B845" s="3" t="s">
-        <v>1676</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A846" s="3" t="s">
-        <v>1677</v>
+        <v>1674</v>
       </c>
       <c r="B846" s="3" t="s">
-        <v>1678</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A847" s="4" t="s">
-        <v>1679</v>
+        <v>1676</v>
       </c>
       <c r="B847" s="4" t="s">
-        <v>1680</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A848" s="3" t="s">
-        <v>1681</v>
+        <v>1678</v>
       </c>
       <c r="B848" s="3" t="s">
-        <v>1682</v>
+        <v>1679</v>
       </c>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A849" s="3" t="s">
-        <v>1683</v>
+        <v>1680</v>
       </c>
       <c r="B849" s="3" t="s">
-        <v>1684</v>
+        <v>1681</v>
       </c>
     </row>
     <row r="850" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A850" s="3" t="s">
-        <v>1685</v>
+        <v>1682</v>
       </c>
       <c r="B850" s="3" t="s">
-        <v>1686</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="851" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A851" s="3" t="s">
-        <v>1687</v>
+        <v>1684</v>
       </c>
       <c r="B851" s="3" t="s">
-        <v>1688</v>
+        <v>1685</v>
       </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A852" s="3" t="s">
-        <v>1689</v>
+        <v>1686</v>
       </c>
       <c r="B852" s="3" t="s">
-        <v>1690</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="853" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A853" s="3" t="s">
-        <v>1691</v>
+        <v>1688</v>
       </c>
       <c r="B853" s="3" t="s">
-        <v>1692</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="854" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A854" s="3" t="s">
-        <v>1693</v>
+        <v>1690</v>
       </c>
       <c r="B854" s="3" t="s">
-        <v>1694</v>
+        <v>1691</v>
       </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A855" s="3" t="s">
-        <v>1695</v>
+        <v>1692</v>
       </c>
       <c r="B855" s="3" t="s">
-        <v>1696</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A856" s="3" t="s">
-        <v>1697</v>
+        <v>1694</v>
       </c>
       <c r="B856" s="3" t="s">
-        <v>1698</v>
+        <v>1695</v>
       </c>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A857" s="3" t="s">
-        <v>1699</v>
+        <v>1696</v>
       </c>
       <c r="B857" s="3" t="s">
-        <v>1700</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="858" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A858" s="3" t="s">
-        <v>1701</v>
+        <v>1698</v>
       </c>
       <c r="B858" s="3" t="s">
-        <v>1702</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="859" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A859" s="3" t="s">
-        <v>1703</v>
+        <v>1700</v>
       </c>
       <c r="B859" s="3" t="s">
-        <v>1704</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="860" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A860" s="3" t="s">
-        <v>1705</v>
+        <v>1702</v>
       </c>
       <c r="B860" s="3" t="s">
-        <v>1706</v>
+        <v>1703</v>
       </c>
     </row>
     <row r="861" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A861" s="3" t="s">
-        <v>1707</v>
+        <v>1704</v>
       </c>
       <c r="B861" s="3" t="s">
-        <v>1708</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="862" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A862" s="4" t="s">
-        <v>1709</v>
+        <v>1706</v>
       </c>
       <c r="B862" s="4" t="s">
-        <v>1710</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="863" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A863" s="3" t="s">
-        <v>1711</v>
+        <v>1708</v>
       </c>
       <c r="B863" s="3" t="s">
-        <v>1712</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="864" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A864" s="3" t="s">
-        <v>1713</v>
+        <v>1710</v>
       </c>
       <c r="B864" s="3" t="s">
-        <v>1714</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="865" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A865" s="3" t="s">
-        <v>1715</v>
+        <v>1712</v>
       </c>
       <c r="B865" s="3" t="s">
-        <v>1716</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="866" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A866" s="3" t="s">
-        <v>1717</v>
+        <v>1714</v>
       </c>
       <c r="B866" s="3" t="s">
-        <v>1718</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="867" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A867" s="3" t="s">
-        <v>1719</v>
+        <v>1716</v>
       </c>
       <c r="B867" s="3" t="s">
-        <v>1720</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="868" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A868" s="3" t="s">
-        <v>1721</v>
+        <v>1718</v>
       </c>
       <c r="B868" s="3" t="s">
-        <v>1722</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="869" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A869" s="3" t="s">
-        <v>1723</v>
+        <v>1720</v>
       </c>
       <c r="B869" s="3" t="s">
-        <v>1724</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="870" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A870" s="3" t="s">
-        <v>1725</v>
+        <v>1722</v>
       </c>
       <c r="B870" s="3" t="s">
-        <v>1726</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="871" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A871" s="3" t="s">
-        <v>1727</v>
+        <v>1724</v>
       </c>
       <c r="B871" s="3" t="s">
-        <v>1728</v>
+        <v>1725</v>
       </c>
     </row>
     <row r="872" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A872" s="3" t="s">
-        <v>1729</v>
+        <v>1726</v>
       </c>
       <c r="B872" s="3" t="s">
-        <v>1730</v>
+        <v>1727</v>
       </c>
     </row>
     <row r="873" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A873" s="3" t="s">
-        <v>1731</v>
+        <v>1728</v>
       </c>
       <c r="B873" s="3" t="s">
-        <v>1732</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="874" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A874" s="3" t="s">
-        <v>1733</v>
+        <v>1730</v>
       </c>
       <c r="B874" s="3" t="s">
-        <v>1734</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="875" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A875" s="4" t="s">
-        <v>1735</v>
+        <v>1732</v>
       </c>
       <c r="B875" s="4" t="s">
-        <v>1736</v>
+        <v>1733</v>
       </c>
     </row>
     <row r="876" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A876" s="3" t="s">
-        <v>1737</v>
+        <v>1734</v>
       </c>
       <c r="B876" s="3" t="s">
-        <v>1738</v>
+        <v>1735</v>
       </c>
     </row>
     <row r="877" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A877" s="3" t="s">
-        <v>1739</v>
+        <v>1736</v>
       </c>
       <c r="B877" s="3" t="s">
-        <v>1740</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="878" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A878" s="3" t="s">
-        <v>1741</v>
+        <v>1738</v>
       </c>
       <c r="B878" s="3" t="s">
-        <v>1742</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="879" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A879" s="3" t="s">
-        <v>1743</v>
+        <v>1740</v>
       </c>
       <c r="B879" s="3" t="s">
-        <v>1744</v>
+        <v>1741</v>
       </c>
     </row>
     <row r="880" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A880" s="3" t="s">
-        <v>1745</v>
+        <v>1742</v>
       </c>
       <c r="B880" s="3" t="s">
-        <v>1746</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="881" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A881" s="3" t="s">
-        <v>1747</v>
+        <v>1744</v>
       </c>
       <c r="B881" s="3" t="s">
-        <v>1748</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="882" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A882" s="3" t="s">
-        <v>1749</v>
+        <v>1746</v>
       </c>
       <c r="B882" s="3" t="s">
-        <v>1750</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="883" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A883" s="3" t="s">
-        <v>1751</v>
+        <v>1748</v>
       </c>
       <c r="B883" s="3" t="s">
-        <v>1752</v>
+        <v>1749</v>
       </c>
     </row>
     <row r="884" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A884" s="3" t="s">
-        <v>1753</v>
+        <v>1750</v>
       </c>
       <c r="B884" s="3" t="s">
-        <v>1754</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="885" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A885" s="3" t="s">
-        <v>1755</v>
+        <v>1752</v>
       </c>
       <c r="B885" s="3" t="s">
-        <v>1756</v>
+        <v>1753</v>
       </c>
     </row>
     <row r="886" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A886" s="3" t="s">
-        <v>1757</v>
+        <v>1754</v>
       </c>
       <c r="B886" s="3" t="s">
-        <v>1758</v>
+        <v>1755</v>
       </c>
     </row>
     <row r="887" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A887" s="3" t="s">
-        <v>1759</v>
+        <v>1756</v>
       </c>
       <c r="B887" s="3" t="s">
-        <v>1760</v>
+        <v>1757</v>
       </c>
     </row>
     <row r="888" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A888" s="3" t="s">
-        <v>1761</v>
+        <v>1758</v>
       </c>
       <c r="B888" s="3" t="s">
-        <v>1762</v>
+        <v>1759</v>
       </c>
     </row>
     <row r="889" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A889" s="3" t="s">
-        <v>1763</v>
+        <v>1760</v>
       </c>
       <c r="B889" s="3" t="s">
-        <v>1764</v>
+        <v>1761</v>
       </c>
     </row>
     <row r="890" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A890" s="3" t="s">
-        <v>1765</v>
+        <v>1762</v>
       </c>
       <c r="B890" s="3" t="s">
-        <v>1766</v>
+        <v>1763</v>
       </c>
     </row>
     <row r="891" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A891" s="3" t="s">
-        <v>1767</v>
+        <v>1764</v>
       </c>
       <c r="B891" s="3" t="s">
-        <v>1768</v>
+        <v>1765</v>
       </c>
     </row>
     <row r="892" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A892" s="3" t="s">
-        <v>1769</v>
+        <v>1766</v>
       </c>
       <c r="B892" s="3" t="s">
-        <v>1770</v>
+        <v>1767</v>
       </c>
     </row>
     <row r="893" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A893" s="3" t="s">
-        <v>1771</v>
+        <v>1768</v>
       </c>
       <c r="B893" s="3" t="s">
-        <v>1772</v>
+        <v>1769</v>
       </c>
     </row>
     <row r="894" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A894" s="3" t="s">
-        <v>1773</v>
+        <v>1770</v>
       </c>
       <c r="B894" s="3" t="s">
-        <v>1774</v>
+        <v>1771</v>
       </c>
     </row>
     <row r="895" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A895" s="7" t="s">
-        <v>1775</v>
+        <v>1772</v>
       </c>
       <c r="B895" s="7" t="s">
-        <v>1776</v>
+        <v>1773</v>
       </c>
     </row>
     <row r="896" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A896" s="3" t="s">
-        <v>1777</v>
+        <v>1774</v>
       </c>
       <c r="B896" s="3" t="s">
-        <v>1778</v>
+        <v>1775</v>
       </c>
     </row>
   </sheetData>

</xml_diff>